<commit_message>
(B)    correct mini blender bottle corrections
</commit_message>
<xml_diff>
--- a/Diet/Suppl/Meal Stats.xlsx
+++ b/Diet/Suppl/Meal Stats.xlsx
@@ -686,9 +686,6 @@
     <t>Opens</t>
   </si>
   <si>
-    <t>Get Smaller Blender Bottle</t>
-  </si>
-  <si>
     <t>Large BB</t>
   </si>
   <si>
@@ -699,6 +696,9 @@
   </si>
   <si>
     <t>X</t>
+  </si>
+  <si>
+    <t>Get Smaller Blender Bottle (20oz. Bottle)</t>
   </si>
 </sst>
 </file>
@@ -1905,6 +1905,73 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="20" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1920,10 +1987,16 @@
     <xf numFmtId="1" fontId="0" fillId="5" borderId="20" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1952,79 +2025,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="17" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="24" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="22" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2309,8 +2309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AQ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="K60" sqref="K60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2431,7 +2431,7 @@
       <c r="AO1" s="43" t="s">
         <v>208</v>
       </c>
-      <c r="AQ1" s="171" t="s">
+      <c r="AQ1" s="155" t="s">
         <v>132</v>
       </c>
     </row>
@@ -2466,7 +2466,7 @@
       <c r="J2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="175" t="s">
+      <c r="K2" s="159" t="s">
         <v>211</v>
       </c>
       <c r="L2" s="131"/>
@@ -2532,11 +2532,11 @@
         <v>113</v>
       </c>
       <c r="AN2" s="142"/>
-      <c r="AO2" s="181" t="s">
+      <c r="AO2" s="164" t="s">
         <v>209</v>
       </c>
       <c r="AQ2" s="47" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="3" spans="1:43" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2558,7 +2558,7 @@
       <c r="F3" s="149">
         <v>12</v>
       </c>
-      <c r="G3" s="189">
+      <c r="G3" s="172">
         <v>2</v>
       </c>
       <c r="H3" s="115">
@@ -2567,15 +2567,15 @@
       <c r="I3" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="185">
+      <c r="J3" s="168">
         <v>6</v>
       </c>
-      <c r="K3" s="176">
+      <c r="K3" s="160">
         <v>1</v>
       </c>
-      <c r="L3" s="193"/>
-      <c r="M3" s="194"/>
-      <c r="N3" s="195"/>
+      <c r="L3" s="175"/>
+      <c r="M3" s="176"/>
+      <c r="N3" s="177"/>
       <c r="O3" s="14"/>
       <c r="Q3" s="42"/>
       <c r="R3" s="42"/>
@@ -2617,7 +2617,7 @@
         <v>0.25</v>
       </c>
       <c r="AN3" s="142"/>
-      <c r="AO3" s="182">
+      <c r="AO3" s="165">
         <v>1</v>
       </c>
     </row>
@@ -2645,7 +2645,7 @@
         <f>R4*$F$3</f>
         <v>216</v>
       </c>
-      <c r="G4" s="190">
+      <c r="G4" s="173">
         <f>$G$3*S4</f>
         <v>240</v>
       </c>
@@ -2653,15 +2653,15 @@
         <f>'Juicer Stats'!M4*$H$3</f>
         <v>319.30537785263732</v>
       </c>
-      <c r="I4" s="174">
+      <c r="I4" s="158">
         <f>AL4*$AL$3+AM4*$AM$3</f>
         <v>31.721999999999998</v>
       </c>
-      <c r="J4" s="186">
+      <c r="J4" s="169">
         <f>$J$3*AO4</f>
         <v>488.40000000000003</v>
       </c>
-      <c r="K4" s="177">
+      <c r="K4" s="161">
         <f>AE4</f>
         <v>120</v>
       </c>
@@ -2738,7 +2738,7 @@
         <v>86.1</v>
       </c>
       <c r="AN4" s="142"/>
-      <c r="AO4" s="182">
+      <c r="AO4" s="165">
         <v>81.400000000000006</v>
       </c>
       <c r="AQ4" s="70">
@@ -2769,24 +2769,24 @@
         <f t="shared" ref="F5:F22" si="4">R5*$F$3</f>
         <v>108</v>
       </c>
-      <c r="G5" s="190">
-        <f t="shared" ref="G5:G19" si="5">$G$3*S5</f>
+      <c r="G5" s="173">
+        <f t="shared" ref="G5:G17" si="5">$G$3*S5</f>
         <v>40</v>
       </c>
       <c r="H5" s="116">
         <f>'Juicer Stats'!M5*$H$3</f>
         <v>15.414954772884617</v>
       </c>
-      <c r="I5" s="174">
+      <c r="I5" s="158">
         <f t="shared" ref="I5:I37" si="6">AL5*$AL$3+AM5*$AM$3</f>
         <v>1.7149999999999999</v>
       </c>
-      <c r="J5" s="186">
+      <c r="J5" s="169">
         <f t="shared" ref="J5:J37" si="7">$J$3*AO5</f>
         <v>300</v>
       </c>
-      <c r="K5" s="177">
-        <f t="shared" ref="K5:K41" si="8">AE5</f>
+      <c r="K5" s="161">
+        <f t="shared" ref="K5:K37" si="8">AE5</f>
         <v>15</v>
       </c>
       <c r="L5" s="25">
@@ -2862,7 +2862,7 @@
         <v>2.9</v>
       </c>
       <c r="AN5" s="142"/>
-      <c r="AO5" s="182">
+      <c r="AO5" s="165">
         <v>50</v>
       </c>
       <c r="AQ5" s="70">
@@ -2893,7 +2893,7 @@
         <f t="shared" si="4"/>
         <v>11.879999999999999</v>
       </c>
-      <c r="G6" s="190">
+      <c r="G6" s="173">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
@@ -2901,15 +2901,15 @@
         <f>'Juicer Stats'!M6*$H$3</f>
         <v>1.6756824652947804</v>
       </c>
-      <c r="I6" s="174">
+      <c r="I6" s="158">
         <f t="shared" si="6"/>
         <v>0.17399999999999999</v>
       </c>
-      <c r="J6" s="186">
+      <c r="J6" s="169">
         <f t="shared" si="7"/>
         <v>33.599999999999994</v>
       </c>
-      <c r="K6" s="177">
+      <c r="K6" s="161">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
@@ -2987,7 +2987,7 @@
         <v>0.3</v>
       </c>
       <c r="AN6" s="142"/>
-      <c r="AO6" s="182">
+      <c r="AO6" s="165">
         <v>5.6</v>
       </c>
       <c r="AQ6" s="70">
@@ -3018,7 +3018,7 @@
         <f t="shared" si="4"/>
         <v>6.8279999999999994</v>
       </c>
-      <c r="G7" s="190">
+      <c r="G7" s="173">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
@@ -3026,15 +3026,15 @@
         <f>'Juicer Stats'!M7*$H$3</f>
         <v>0.32329020660659347</v>
       </c>
-      <c r="I7" s="174">
+      <c r="I7" s="158">
         <f t="shared" si="6"/>
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="J7" s="186">
+      <c r="J7" s="169">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="K7" s="177">
+      <c r="K7" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3112,7 +3112,7 @@
         <v>0.1</v>
       </c>
       <c r="AN7" s="142"/>
-      <c r="AO7" s="182">
+      <c r="AO7" s="165">
         <v>1</v>
       </c>
       <c r="AQ7" s="70">
@@ -3140,18 +3140,18 @@
       <c r="F8" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G8" s="190" t="s">
+      <c r="G8" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H8" s="116">
         <f>'Juicer Stats'!M8*$H$3</f>
         <v>0</v>
       </c>
-      <c r="I8" s="174"/>
-      <c r="J8" s="186" t="s">
-        <v>37</v>
-      </c>
-      <c r="K8" s="177">
+      <c r="I8" s="158"/>
+      <c r="J8" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="K8" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3227,7 +3227,7 @@
         <v>37</v>
       </c>
       <c r="AN8" s="142"/>
-      <c r="AO8" s="182" t="s">
+      <c r="AO8" s="165" t="s">
         <v>37</v>
       </c>
       <c r="AQ8" s="70">
@@ -3258,22 +3258,22 @@
         <f t="shared" si="4"/>
         <v>0.70799999999999996</v>
       </c>
-      <c r="G9" s="190" t="s">
+      <c r="G9" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H9" s="116">
         <f>'Juicer Stats'!M9*$H$3</f>
         <v>0.76138921410659344</v>
       </c>
-      <c r="I9" s="174">
+      <c r="I9" s="158">
         <f t="shared" si="6"/>
         <v>0.05</v>
       </c>
-      <c r="J9" s="186">
+      <c r="J9" s="169">
         <f t="shared" si="7"/>
         <v>8.3999999999999986</v>
       </c>
-      <c r="K9" s="177">
+      <c r="K9" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3351,7 +3351,7 @@
         <v>0.2</v>
       </c>
       <c r="AN9" s="142"/>
-      <c r="AO9" s="182">
+      <c r="AO9" s="165">
         <v>1.4</v>
       </c>
       <c r="AQ9" s="70">
@@ -3382,22 +3382,22 @@
         <f t="shared" si="4"/>
         <v>2.976</v>
       </c>
-      <c r="G10" s="190" t="s">
+      <c r="G10" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H10" s="116">
         <f>'Juicer Stats'!M10*$H$3</f>
         <v>0.33</v>
       </c>
-      <c r="I10" s="174">
+      <c r="I10" s="158">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J10" s="186">
+      <c r="J10" s="169">
         <f t="shared" si="7"/>
         <v>14.399999999999999</v>
       </c>
-      <c r="K10" s="177">
+      <c r="K10" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>0</v>
       </c>
       <c r="AN10" s="142"/>
-      <c r="AO10" s="182">
+      <c r="AO10" s="165">
         <v>2.4</v>
       </c>
       <c r="AQ10" s="70">
@@ -3504,19 +3504,19 @@
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="G11" s="190" t="s">
+      <c r="G11" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H11" s="116">
         <f>'Juicer Stats'!M11*$H$3</f>
         <v>0</v>
       </c>
-      <c r="I11" s="174"/>
-      <c r="J11" s="186">
+      <c r="I11" s="158"/>
+      <c r="J11" s="169">
         <f t="shared" si="7"/>
         <v>73.199999999999989</v>
       </c>
-      <c r="K11" s="177">
+      <c r="K11" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -3592,7 +3592,7 @@
         <v>37</v>
       </c>
       <c r="AN11" s="142"/>
-      <c r="AO11" s="182">
+      <c r="AO11" s="165">
         <v>12.2</v>
       </c>
       <c r="AQ11" s="70">
@@ -3623,27 +3623,27 @@
         <f t="shared" si="4"/>
         <v>144</v>
       </c>
-      <c r="G12" s="190" t="s">
+      <c r="G12" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H12" s="116">
         <f>'Juicer Stats'!M12*$H$3</f>
         <v>73.584356356318679</v>
       </c>
-      <c r="I12" s="174">
+      <c r="I12" s="158">
         <f t="shared" si="6"/>
         <v>57.875</v>
       </c>
-      <c r="J12" s="186">
+      <c r="J12" s="169">
         <f t="shared" si="7"/>
         <v>904.80000000000007</v>
       </c>
-      <c r="K12" s="177">
+      <c r="K12" s="161">
         <f t="shared" si="8"/>
         <v>180</v>
       </c>
       <c r="L12" s="25">
-        <f t="shared" ref="L5:L37" si="12">SUM(B12:K12)</f>
+        <f t="shared" ref="L12:L17" si="12">SUM(B12:K12)</f>
         <v>3088.8926896896523</v>
       </c>
       <c r="M12" s="24">
@@ -3714,7 +3714,7 @@
         <v>191.9</v>
       </c>
       <c r="AN12" s="142"/>
-      <c r="AO12" s="182">
+      <c r="AO12" s="165">
         <v>150.80000000000001</v>
       </c>
       <c r="AQ12" s="70">
@@ -3745,22 +3745,22 @@
         <f t="shared" si="4"/>
         <v>528</v>
       </c>
-      <c r="G13" s="190" t="s">
+      <c r="G13" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H13" s="116">
         <f>'Juicer Stats'!M13*$H$3</f>
         <v>892.22522370263744</v>
       </c>
-      <c r="I13" s="174">
+      <c r="I13" s="158">
         <f t="shared" si="6"/>
         <v>240.65800000000002</v>
       </c>
-      <c r="J13" s="186">
+      <c r="J13" s="169">
         <f t="shared" si="7"/>
         <v>444</v>
       </c>
-      <c r="K13" s="177">
+      <c r="K13" s="161">
         <f t="shared" si="8"/>
         <v>115</v>
       </c>
@@ -3835,7 +3835,7 @@
         <v>583</v>
       </c>
       <c r="AN13" s="142"/>
-      <c r="AO13" s="182">
+      <c r="AO13" s="165">
         <v>74</v>
       </c>
       <c r="AQ13" s="70">
@@ -3866,7 +3866,7 @@
         <f t="shared" si="4"/>
         <v>16.559999999999999</v>
       </c>
-      <c r="G14" s="190">
+      <c r="G14" s="173">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
@@ -3874,15 +3874,15 @@
         <f>'Juicer Stats'!M14*$H$3</f>
         <v>73.867640943654948</v>
       </c>
-      <c r="I14" s="174">
+      <c r="I14" s="158">
         <f t="shared" si="6"/>
         <v>7.0549999999999997</v>
       </c>
-      <c r="J14" s="186">
+      <c r="J14" s="169">
         <f t="shared" si="7"/>
         <v>21.6</v>
       </c>
-      <c r="K14" s="177">
+      <c r="K14" s="161">
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
@@ -3960,7 +3960,7 @@
         <v>20.3</v>
       </c>
       <c r="AN14" s="142"/>
-      <c r="AO14" s="182">
+      <c r="AO14" s="165">
         <v>3.6</v>
       </c>
       <c r="AQ14" s="70">
@@ -3991,22 +3991,22 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G15" s="190" t="s">
+      <c r="G15" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H15" s="116">
         <f>'Juicer Stats'!M15*$H$3</f>
         <v>13.631067231390112</v>
       </c>
-      <c r="I15" s="174">
+      <c r="I15" s="158">
         <f t="shared" si="6"/>
         <v>2.5670000000000002</v>
       </c>
-      <c r="J15" s="186">
+      <c r="J15" s="169">
         <f t="shared" si="7"/>
         <v>0.60000000000000009</v>
       </c>
-      <c r="K15" s="177">
+      <c r="K15" s="161">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
@@ -4084,7 +4084,7 @@
         <v>7.1</v>
       </c>
       <c r="AN15" s="142"/>
-      <c r="AO15" s="182">
+      <c r="AO15" s="165">
         <v>0.1</v>
       </c>
       <c r="AQ15" s="70">
@@ -4115,7 +4115,7 @@
         <f t="shared" si="4"/>
         <v>19.200000000000003</v>
       </c>
-      <c r="G16" s="190">
+      <c r="G16" s="173">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
@@ -4123,15 +4123,15 @@
         <f>'Juicer Stats'!M16*$H$3</f>
         <v>22.559373536171154</v>
       </c>
-      <c r="I16" s="174">
+      <c r="I16" s="158">
         <f t="shared" si="6"/>
         <v>3.42</v>
       </c>
-      <c r="J16" s="186">
+      <c r="J16" s="169">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K16" s="177">
+      <c r="K16" s="161">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
@@ -4209,7 +4209,7 @@
         <v>11.7</v>
       </c>
       <c r="AN16" s="142"/>
-      <c r="AO16" s="182">
+      <c r="AO16" s="165">
         <v>0</v>
       </c>
       <c r="AQ16" s="70">
@@ -4240,7 +4240,7 @@
         <f t="shared" si="4"/>
         <v>11.76</v>
       </c>
-      <c r="G17" s="190">
+      <c r="G17" s="173">
         <f t="shared" si="5"/>
         <v>48</v>
       </c>
@@ -4248,15 +4248,15 @@
         <f>'Juicer Stats'!M17*$H$3</f>
         <v>8.560484252507969</v>
       </c>
-      <c r="I17" s="174">
+      <c r="I17" s="158">
         <f t="shared" si="6"/>
         <v>1.258</v>
       </c>
-      <c r="J17" s="186">
+      <c r="J17" s="169">
         <f t="shared" si="7"/>
         <v>25.200000000000003</v>
       </c>
-      <c r="K17" s="177">
+      <c r="K17" s="161">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
@@ -4333,7 +4333,7 @@
         <v>1.6</v>
       </c>
       <c r="AN17" s="142"/>
-      <c r="AO17" s="182">
+      <c r="AO17" s="165">
         <v>4.2</v>
       </c>
       <c r="AQ17" s="70">
@@ -4342,16 +4342,16 @@
     </row>
     <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
-      <c r="B18" s="155"/>
-      <c r="C18" s="156"/>
-      <c r="D18" s="157"/>
-      <c r="E18" s="158"/>
-      <c r="F18" s="159"/>
-      <c r="G18" s="191"/>
+      <c r="B18" s="178"/>
+      <c r="C18" s="179"/>
+      <c r="D18" s="180"/>
+      <c r="E18" s="181"/>
+      <c r="F18" s="182"/>
+      <c r="G18" s="183"/>
       <c r="H18" s="116"/>
-      <c r="I18" s="160"/>
-      <c r="J18" s="161"/>
-      <c r="K18" s="178"/>
+      <c r="I18" s="184"/>
+      <c r="J18" s="185"/>
+      <c r="K18" s="186"/>
       <c r="L18" s="32"/>
       <c r="M18" s="33"/>
       <c r="N18" s="34"/>
@@ -4390,7 +4390,7 @@
       <c r="AL18" s="119"/>
       <c r="AM18" s="20"/>
       <c r="AN18" s="142"/>
-      <c r="AO18" s="182"/>
+      <c r="AO18" s="165"/>
       <c r="AQ18" s="70"/>
     </row>
     <row r="19" spans="1:43" x14ac:dyDescent="0.25">
@@ -4417,22 +4417,22 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-      <c r="G19" s="190" t="s">
+      <c r="G19" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H19" s="116">
         <f>'Juicer Stats'!M19*$H$3</f>
         <v>48.128538775799264</v>
       </c>
-      <c r="I19" s="174">
+      <c r="I19" s="158">
         <f t="shared" si="6"/>
         <v>48.57</v>
       </c>
-      <c r="J19" s="186">
+      <c r="J19" s="169">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K19" s="177">
+      <c r="K19" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4508,7 +4508,7 @@
         <v>189</v>
       </c>
       <c r="AN19" s="142"/>
-      <c r="AO19" s="182">
+      <c r="AO19" s="165">
         <v>0</v>
       </c>
       <c r="AQ19" s="70">
@@ -4539,22 +4539,22 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G20" s="190" t="s">
+      <c r="G20" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H20" s="116">
         <f>'Juicer Stats'!M20*$H$3</f>
         <v>136.07938444967309</v>
       </c>
-      <c r="I20" s="174">
+      <c r="I20" s="158">
         <f t="shared" si="6"/>
         <v>47.63</v>
       </c>
-      <c r="J20" s="186">
+      <c r="J20" s="169">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="K20" s="177">
+      <c r="K20" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4628,7 +4628,7 @@
         <v>11</v>
       </c>
       <c r="AN20" s="142"/>
-      <c r="AO20" s="182">
+      <c r="AO20" s="165">
         <v>0</v>
       </c>
       <c r="AQ20" s="70">
@@ -4659,22 +4659,22 @@
         <f t="shared" si="4"/>
         <v>36</v>
       </c>
-      <c r="G21" s="190" t="s">
+      <c r="G21" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H21" s="116">
         <f>'Juicer Stats'!M21*$H$3</f>
         <v>11.551983741769368</v>
       </c>
-      <c r="I21" s="174">
+      <c r="I21" s="158">
         <f t="shared" si="6"/>
         <v>3.6500000000000004</v>
       </c>
-      <c r="J21" s="186">
+      <c r="J21" s="169">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="K21" s="177">
+      <c r="K21" s="161">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
@@ -4750,7 +4750,7 @@
         <v>8</v>
       </c>
       <c r="AN21" s="142"/>
-      <c r="AO21" s="182">
+      <c r="AO21" s="165">
         <v>1</v>
       </c>
       <c r="AQ21" s="70">
@@ -4781,22 +4781,22 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="G22" s="190" t="s">
+      <c r="G22" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H22" s="116">
         <f>'Juicer Stats'!M22*$H$3</f>
         <v>28.559650157197805</v>
       </c>
-      <c r="I22" s="174">
+      <c r="I22" s="158">
         <f t="shared" si="6"/>
         <v>9.9700000000000006</v>
       </c>
-      <c r="J22" s="186">
+      <c r="J22" s="169">
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="K22" s="177">
+      <c r="K22" s="161">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
@@ -4872,7 +4872,7 @@
         <v>28</v>
       </c>
       <c r="AN22" s="142"/>
-      <c r="AO22" s="182">
+      <c r="AO22" s="165">
         <v>4</v>
       </c>
       <c r="AQ22" s="70">
@@ -4900,22 +4900,22 @@
       <c r="F23" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="190" t="s">
+      <c r="G23" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H23" s="116">
         <f>'Juicer Stats'!M23*$H$3</f>
         <v>38.774999999999999</v>
       </c>
-      <c r="I23" s="174">
+      <c r="I23" s="158">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J23" s="186">
+      <c r="J23" s="169">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="K23" s="177">
+      <c r="K23" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -4989,7 +4989,7 @@
         <v>0</v>
       </c>
       <c r="AN23" s="142"/>
-      <c r="AO23" s="182">
+      <c r="AO23" s="165">
         <v>1</v>
       </c>
       <c r="AQ23" s="70">
@@ -5016,22 +5016,22 @@
       <c r="F24" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G24" s="190" t="s">
+      <c r="G24" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H24" s="116">
         <f>'Juicer Stats'!M24*$H$3</f>
         <v>45.081313256897801</v>
       </c>
-      <c r="I24" s="174">
+      <c r="I24" s="158">
         <f>AL24*$AL$3</f>
         <v>1.6500000000000001</v>
       </c>
-      <c r="J24" s="186">
+      <c r="J24" s="169">
         <f t="shared" si="7"/>
         <v>18</v>
       </c>
-      <c r="K24" s="177">
+      <c r="K24" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -5107,7 +5107,7 @@
         <v>37</v>
       </c>
       <c r="AN24" s="142"/>
-      <c r="AO24" s="182">
+      <c r="AO24" s="165">
         <v>3</v>
       </c>
       <c r="AQ24" s="70">
@@ -5134,22 +5134,22 @@
       <c r="F25" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G25" s="190" t="s">
+      <c r="G25" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H25" s="116">
         <f>'Juicer Stats'!M25*$H$3</f>
         <v>101.34643885179499</v>
       </c>
-      <c r="I25" s="174">
+      <c r="I25" s="158">
         <f t="shared" si="6"/>
         <v>30.740000000000002</v>
       </c>
-      <c r="J25" s="186">
+      <c r="J25" s="169">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="K25" s="177">
+      <c r="K25" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -5225,7 +5225,7 @@
         <v>20</v>
       </c>
       <c r="AN25" s="142"/>
-      <c r="AO25" s="182">
+      <c r="AO25" s="165">
         <v>1</v>
       </c>
       <c r="AQ25" s="70">
@@ -5253,22 +5253,22 @@
       <c r="F26" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G26" s="190" t="s">
+      <c r="G26" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H26" s="116">
         <f>'Juicer Stats'!M26*$H$3</f>
         <v>47.165179434697812</v>
       </c>
-      <c r="I26" s="174">
+      <c r="I26" s="158">
         <f t="shared" si="6"/>
         <v>2.9000000000000004</v>
       </c>
-      <c r="J26" s="186">
+      <c r="J26" s="169">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="K26" s="177">
+      <c r="K26" s="161">
         <f t="shared" si="8"/>
         <v>15</v>
       </c>
@@ -5344,7 +5344,7 @@
         <v>5</v>
       </c>
       <c r="AN26" s="142"/>
-      <c r="AO26" s="182">
+      <c r="AO26" s="165">
         <v>2</v>
       </c>
       <c r="AQ26" s="70">
@@ -5372,22 +5372,22 @@
       <c r="F27" s="154" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="190" t="s">
+      <c r="G27" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H27" s="116">
         <f>'Juicer Stats'!M27*$H$3</f>
         <v>42.927936076263741</v>
       </c>
-      <c r="I27" s="174">
+      <c r="I27" s="158">
         <f t="shared" si="6"/>
         <v>3.81</v>
       </c>
-      <c r="J27" s="186">
+      <c r="J27" s="169">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="K27" s="177">
+      <c r="K27" s="161">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
@@ -5463,7 +5463,7 @@
         <v>6</v>
       </c>
       <c r="AN27" s="142"/>
-      <c r="AO27" s="182">
+      <c r="AO27" s="165">
         <v>2</v>
       </c>
       <c r="AQ27" s="70">
@@ -5491,22 +5491,22 @@
       <c r="F28" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="190" t="s">
+      <c r="G28" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H28" s="116">
         <f>'Juicer Stats'!M28*$H$3</f>
         <v>26.126536544065932</v>
       </c>
-      <c r="I28" s="174">
+      <c r="I28" s="158">
         <f t="shared" si="6"/>
         <v>3.0700000000000003</v>
       </c>
-      <c r="J28" s="186">
+      <c r="J28" s="169">
         <f t="shared" si="7"/>
         <v>42</v>
       </c>
-      <c r="K28" s="177">
+      <c r="K28" s="161">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>7</v>
       </c>
       <c r="AN28" s="142"/>
-      <c r="AO28" s="182">
+      <c r="AO28" s="165">
         <v>7</v>
       </c>
       <c r="AQ28" s="70">
@@ -5610,22 +5610,22 @@
       <c r="F29" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G29" s="190" t="s">
+      <c r="G29" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H29" s="116">
         <f>'Juicer Stats'!M29*$H$3</f>
         <v>58.803024306895608</v>
       </c>
-      <c r="I29" s="174">
+      <c r="I29" s="158">
         <f t="shared" si="6"/>
         <v>11.54</v>
       </c>
-      <c r="J29" s="186">
+      <c r="J29" s="169">
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="K29" s="177">
+      <c r="K29" s="161">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
@@ -5699,7 +5699,7 @@
         <v>29</v>
       </c>
       <c r="AN29" s="142"/>
-      <c r="AO29" s="182">
+      <c r="AO29" s="165">
         <v>4</v>
       </c>
       <c r="AQ29" s="70">
@@ -5726,22 +5726,22 @@
       <c r="F30" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G30" s="190" t="s">
+      <c r="G30" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H30" s="116">
         <f>'Juicer Stats'!M30*$H$3</f>
         <v>35.704672180631874</v>
       </c>
-      <c r="I30" s="174">
+      <c r="I30" s="158">
         <f t="shared" si="6"/>
         <v>9.1999999999999993</v>
       </c>
-      <c r="J30" s="186">
+      <c r="J30" s="169">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="K30" s="177">
+      <c r="K30" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -5815,7 +5815,7 @@
         <v>17</v>
       </c>
       <c r="AN30" s="142"/>
-      <c r="AO30" s="182">
+      <c r="AO30" s="165">
         <v>1</v>
       </c>
       <c r="AQ30" s="70">
@@ -5843,22 +5843,22 @@
       <c r="F31" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G31" s="190" t="s">
+      <c r="G31" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H31" s="116">
         <f>'Juicer Stats'!M31*$H$3</f>
         <v>49.5</v>
       </c>
-      <c r="I31" s="174">
+      <c r="I31" s="158">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="J31" s="186">
+      <c r="J31" s="169">
         <f t="shared" si="7"/>
         <v>24</v>
       </c>
-      <c r="K31" s="177">
+      <c r="K31" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -5930,7 +5930,7 @@
         <v>0</v>
       </c>
       <c r="AN31" s="142"/>
-      <c r="AO31" s="182">
+      <c r="AO31" s="165">
         <v>4</v>
       </c>
       <c r="AQ31" s="70">
@@ -5957,18 +5957,18 @@
       <c r="F32" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G32" s="190" t="s">
+      <c r="G32" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H32" s="116">
         <f>'Juicer Stats'!M32*$H$3</f>
         <v>38.774999999999999</v>
       </c>
-      <c r="I32" s="174"/>
-      <c r="J32" s="186" t="s">
-        <v>37</v>
-      </c>
-      <c r="K32" s="177">
+      <c r="I32" s="158"/>
+      <c r="J32" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="K32" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -6036,7 +6036,7 @@
         <v>37</v>
       </c>
       <c r="AN32" s="142"/>
-      <c r="AO32" s="182" t="s">
+      <c r="AO32" s="165" t="s">
         <v>37</v>
       </c>
       <c r="AQ32" s="70">
@@ -6063,18 +6063,18 @@
       <c r="F33" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G33" s="190" t="s">
+      <c r="G33" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H33" s="116">
         <f>'Juicer Stats'!M33*$H$3</f>
         <v>22.362731453065386</v>
       </c>
-      <c r="I33" s="174"/>
-      <c r="J33" s="186" t="s">
-        <v>37</v>
-      </c>
-      <c r="K33" s="177">
+      <c r="I33" s="158"/>
+      <c r="J33" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" s="161">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
@@ -6144,7 +6144,7 @@
         <v>37</v>
       </c>
       <c r="AN33" s="142"/>
-      <c r="AO33" s="182" t="s">
+      <c r="AO33" s="165" t="s">
         <v>37</v>
       </c>
       <c r="AQ33" s="70">
@@ -6171,22 +6171,22 @@
       <c r="F34" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="190" t="s">
+      <c r="G34" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H34" s="116">
         <f>'Juicer Stats'!M34*$H$3</f>
         <v>26.798572734697807</v>
       </c>
-      <c r="I34" s="174">
+      <c r="I34" s="158">
         <f t="shared" si="6"/>
         <v>4.0600000000000005</v>
       </c>
-      <c r="J34" s="186">
+      <c r="J34" s="169">
         <f t="shared" si="7"/>
         <v>36</v>
       </c>
-      <c r="K34" s="177">
+      <c r="K34" s="161">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
@@ -6262,7 +6262,7 @@
         <v>7</v>
       </c>
       <c r="AN34" s="142"/>
-      <c r="AO34" s="182">
+      <c r="AO34" s="165">
         <v>6</v>
       </c>
       <c r="AQ34" s="70">
@@ -6289,18 +6289,18 @@
       <c r="F35" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="190" t="s">
+      <c r="G35" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H35" s="116">
         <f>'Juicer Stats'!M35*$H$3</f>
         <v>0</v>
       </c>
-      <c r="I35" s="174"/>
-      <c r="J35" s="186" t="s">
-        <v>37</v>
-      </c>
-      <c r="K35" s="177">
+      <c r="I35" s="158"/>
+      <c r="J35" s="169" t="s">
+        <v>37</v>
+      </c>
+      <c r="K35" s="161">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
@@ -6368,7 +6368,7 @@
         <v>0</v>
       </c>
       <c r="AN35" s="142"/>
-      <c r="AO35" s="182" t="s">
+      <c r="AO35" s="165" t="s">
         <v>37</v>
       </c>
       <c r="AQ35" s="70">
@@ -6395,22 +6395,22 @@
       <c r="F36" s="151" t="s">
         <v>37</v>
       </c>
-      <c r="G36" s="190" t="s">
+      <c r="G36" s="173" t="s">
         <v>37</v>
       </c>
       <c r="H36" s="116">
         <f>'Juicer Stats'!M36*$H$3</f>
         <v>46.733592427197806</v>
       </c>
-      <c r="I36" s="174">
+      <c r="I36" s="158">
         <f t="shared" si="6"/>
         <v>3.98</v>
       </c>
-      <c r="J36" s="186">
+      <c r="J36" s="169">
         <f t="shared" si="7"/>
         <v>12</v>
       </c>
-      <c r="K36" s="177">
+      <c r="K36" s="161">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
@@ -6487,7 +6487,7 @@
         <v>8</v>
       </c>
       <c r="AN36" s="142"/>
-      <c r="AO36" s="182">
+      <c r="AO36" s="165">
         <v>2</v>
       </c>
       <c r="AQ36" s="70">
@@ -6514,22 +6514,22 @@
       <c r="F37" s="153" t="s">
         <v>37</v>
       </c>
-      <c r="G37" s="192" t="s">
+      <c r="G37" s="174" t="s">
         <v>37</v>
       </c>
       <c r="H37" s="117">
         <f>'Juicer Stats'!M37*$H$3</f>
         <v>67.289897540499993</v>
       </c>
-      <c r="I37" s="179">
+      <c r="I37" s="162">
         <f t="shared" si="6"/>
         <v>2.3200000000000003</v>
       </c>
-      <c r="J37" s="187">
+      <c r="J37" s="170">
         <f t="shared" si="7"/>
         <v>60</v>
       </c>
-      <c r="K37" s="180">
+      <c r="K37" s="163">
         <f t="shared" si="8"/>
         <v>20</v>
       </c>
@@ -6591,7 +6591,7 @@
       </c>
       <c r="AH37" s="121"/>
       <c r="AI37" s="141"/>
-      <c r="AJ37" s="172">
+      <c r="AJ37" s="156">
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
@@ -6599,11 +6599,11 @@
       <c r="AL37" s="120">
         <v>4</v>
       </c>
-      <c r="AM37" s="173">
+      <c r="AM37" s="157">
         <v>4</v>
       </c>
       <c r="AN37" s="142"/>
-      <c r="AO37" s="183">
+      <c r="AO37" s="166">
         <v>10</v>
       </c>
       <c r="AQ37" s="70">
@@ -6615,11 +6615,11 @@
       <c r="I38" s="42"/>
       <c r="J38" s="42"/>
       <c r="K38" s="42"/>
-      <c r="L38" s="162" t="s">
+      <c r="L38" s="187" t="s">
         <v>69</v>
       </c>
-      <c r="M38" s="163"/>
-      <c r="N38" s="164"/>
+      <c r="M38" s="188"/>
+      <c r="N38" s="189"/>
       <c r="O38" s="106"/>
       <c r="P38" s="112" t="s">
         <v>37</v>
@@ -6716,7 +6716,7 @@
       <c r="AN40" s="75" t="s">
         <v>102</v>
       </c>
-      <c r="AO40" s="184" t="s">
+      <c r="AO40" s="167" t="s">
         <v>210</v>
       </c>
       <c r="AP40" t="s">
@@ -6894,7 +6894,7 @@
         <v>161</v>
       </c>
       <c r="J54" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K54" t="s">
         <v>214</v>
@@ -6909,7 +6909,7 @@
         <v>162</v>
       </c>
       <c r="J55" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K55" t="s">
         <v>215</v>
@@ -6925,7 +6925,7 @@
         <v>163</v>
       </c>
       <c r="J56" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K56" t="s">
         <v>216</v>
@@ -6943,7 +6943,7 @@
       <c r="A58" s="90" t="s">
         <v>171</v>
       </c>
-      <c r="K58" s="188" t="s">
+      <c r="K58" s="171" t="s">
         <v>220</v>
       </c>
       <c r="X58" s="112"/>
@@ -6954,14 +6954,14 @@
         <v>132</v>
       </c>
       <c r="K59" s="85" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="X59" s="112"/>
     </row>
     <row r="60" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A60" s="90"/>
       <c r="K60" s="85" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="X60" s="112"/>
     </row>
@@ -6970,7 +6970,7 @@
         <v>164</v>
       </c>
       <c r="K61" s="85" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="X61" s="112"/>
     </row>
@@ -8515,29 +8515,29 @@
     </row>
     <row r="18" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A18" s="18"/>
-      <c r="B18" s="168"/>
-      <c r="C18" s="169"/>
-      <c r="D18" s="169"/>
-      <c r="E18" s="169"/>
-      <c r="F18" s="169"/>
-      <c r="G18" s="169"/>
-      <c r="H18" s="169"/>
-      <c r="I18" s="169"/>
-      <c r="J18" s="169"/>
-      <c r="K18" s="170"/>
+      <c r="B18" s="193"/>
+      <c r="C18" s="194"/>
+      <c r="D18" s="194"/>
+      <c r="E18" s="194"/>
+      <c r="F18" s="194"/>
+      <c r="G18" s="194"/>
+      <c r="H18" s="194"/>
+      <c r="I18" s="194"/>
+      <c r="J18" s="194"/>
+      <c r="K18" s="195"/>
       <c r="L18" s="32"/>
       <c r="M18" s="99"/>
       <c r="Q18" s="18"/>
-      <c r="R18" s="165"/>
-      <c r="S18" s="166"/>
-      <c r="T18" s="166"/>
-      <c r="U18" s="166"/>
-      <c r="V18" s="166"/>
-      <c r="W18" s="166"/>
-      <c r="X18" s="166"/>
-      <c r="Y18" s="166"/>
-      <c r="Z18" s="166"/>
-      <c r="AA18" s="167"/>
+      <c r="R18" s="190"/>
+      <c r="S18" s="191"/>
+      <c r="T18" s="191"/>
+      <c r="U18" s="191"/>
+      <c r="V18" s="191"/>
+      <c r="W18" s="191"/>
+      <c r="X18" s="191"/>
+      <c r="Y18" s="191"/>
+      <c r="Z18" s="191"/>
+      <c r="AA18" s="192"/>
       <c r="AB18" s="45"/>
       <c r="AC18" s="76"/>
     </row>

</xml_diff>